<commit_message>
Selenium Session - 07Aug
</commit_message>
<xml_diff>
--- a/resources/testData.xlsx
+++ b/resources/testData.xlsx
@@ -12,11 +12,12 @@
     <sheet name="RunnerConfig" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:Q25"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>DEL</t>
   </si>
@@ -97,6 +98,18 @@
   </si>
   <si>
     <t>Login to Flipkart</t>
+  </si>
+  <si>
+    <t>TestCase 01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Case02 </t>
+  </si>
+  <si>
+    <t>testCase01</t>
+  </si>
+  <si>
+    <t>testCase02</t>
   </si>
 </sst>
 </file>
@@ -588,10 +601,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -628,7 +641,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -645,7 +658,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D3" s="1">
         <v>2</v>
@@ -662,7 +675,7 @@
         <v>25</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D4" s="1">
         <v>3</v>
@@ -680,6 +693,28 @@
       </c>
       <c r="C5" s="5" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>